<commit_message>
Agrandissement du terrain + design graphique des objectifs et montagnes
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Rois\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CE1CD8-0955-44B9-ADFC-D3546A0A18CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A29F88C-C564-460B-A717-B9924C2E7EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Dé</t>
   </si>
@@ -72,7 +72,10 @@
     <t>7/joueurs</t>
   </si>
   <si>
-    <t>19/joueurs*3</t>
+    <t>37/joueurs*3</t>
+  </si>
+  <si>
+    <t>0.5*37/joueurs*4</t>
   </si>
 </sst>
 </file>
@@ -710,15 +713,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37527EB6-6690-4DE5-953A-72CFC0535AC8}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,19 +757,37 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <f>19/B1*3</f>
-        <v>28.5</v>
+        <f>37/B1*3</f>
+        <v>55.5</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:D4" si="0">19/C1*3</f>
-        <v>19</v>
+        <f t="shared" ref="C4:D4" si="0">37/C1*3</f>
+        <v>37</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>14.25</v>
+        <v>27.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <f>0.5*B4</f>
+        <v>27.75</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:D5" si="1">0.5*C4</f>
+        <v>18.5</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>13.875</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remplacement des montagnes par des hexagones retirés
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A29F88C-C564-460B-A717-B9924C2E7EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B800A976-6472-4842-8C1F-C20EAC3AD21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recrutement" sheetId="1" r:id="rId1"/>
     <sheet name="Saboteurs" sheetId="2" r:id="rId2"/>
-    <sheet name="Montagnes" sheetId="3" r:id="rId3"/>
+    <sheet name="Obstacles" sheetId="3" r:id="rId3"/>
     <sheet name="Cibles" sheetId="4" r:id="rId4"/>
     <sheet name="Troupes" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -63,9 +63,6 @@
     <t>Saboteurs</t>
   </si>
   <si>
-    <t>Montagnes</t>
-  </si>
-  <si>
     <t>Cibles</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>0.5*37/joueurs*4</t>
+  </si>
+  <si>
+    <t>Obstacles</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CA0E9F-C7C5-4402-B952-FCA0B456B247}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>4</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <f>7/B1</f>
@@ -715,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37527EB6-6690-4DE5-953A-72CFC0535AC8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -754,7 +754,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <f>37/B1*3</f>
@@ -771,7 +771,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <f>0.5*B4</f>

</xml_diff>

<commit_message>
design graphiques des tuiles et des cartes
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B800A976-6472-4842-8C1F-C20EAC3AD21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2382F1A-0CC4-470C-8C58-6E9B971B1720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recrutement" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Obstacles" sheetId="3" r:id="rId3"/>
     <sheet name="Cibles" sheetId="4" r:id="rId4"/>
     <sheet name="Troupes" sheetId="5" r:id="rId5"/>
+    <sheet name="Dimensios" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Dé</t>
   </si>
@@ -76,14 +77,39 @@
   </si>
   <si>
     <t>Obstacles</t>
+  </si>
+  <si>
+    <t>hauteur [cm]</t>
+  </si>
+  <si>
+    <t>largeur [cm]</t>
+  </si>
+  <si>
+    <t>facteur</t>
+  </si>
+  <si>
+    <t>Mais les paramètres "hauteur" et "largeur"</t>
+  </si>
+  <si>
+    <t>ne semblent pas ce que je crois</t>
+  </si>
+  <si>
+    <t>Donc, ma méthode de construction d'un hexgagone régulier</t>
+  </si>
+  <si>
+    <t>va plutôt passer par l'ajustement à la main</t>
+  </si>
+  <si>
+    <t>d'un cercle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -167,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +213,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,6 +237,138 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>58540</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>91582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>593482</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>146538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Hexagone 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43BD0124-D694-11A4-E2CE-FAE1C6083238}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3890521" y="282082"/>
+          <a:ext cx="2820942" cy="2531456"/>
+        </a:xfrm>
+        <a:prstGeom prst="hexagon">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209217</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90837</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>443217</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>129444</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Ellipse 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D5CBE63-7C68-002F-7596-EDF1F8BF6840}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4041629" y="281337"/>
+          <a:ext cx="2520000" cy="2515107"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CA0E9F-C7C5-4402-B952-FCA0B456B247}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -790,4 +957,74 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4EFBF6-12B3-45D8-B982-5090B8A756CF}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7">
+        <f>B1*B3</f>
+        <v>8.0829037686547593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8">
+        <f>2*SQRT(3)/3</f>
+        <v>1.1547005383792515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mis à jour en cours
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2382F1A-0CC4-470C-8C58-6E9B971B1720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD71542-E16F-4E2C-A456-86D4EF597EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recrutement" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Obstacles" sheetId="3" r:id="rId3"/>
     <sheet name="Cibles" sheetId="4" r:id="rId4"/>
     <sheet name="Troupes" sheetId="5" r:id="rId5"/>
-    <sheet name="Dimensios" sheetId="6" r:id="rId6"/>
+    <sheet name="Dimensions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -219,7 +219,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -737,7 +737,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,8 +766,8 @@
       <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2" s="6">
-        <v>1</v>
+      <c r="D2" s="5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CA0E9F-C7C5-4402-B952-FCA0B456B247}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -963,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4EFBF6-12B3-45D8-B982-5090B8A756CF}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Amélioration de la rédaction de la règle du dernier tour
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD71542-E16F-4E2C-A456-86D4EF597EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3CF269-AF03-4083-9FFC-8CFAE06E55FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Recrutement" sheetId="1" r:id="rId1"/>
-    <sheet name="Saboteurs" sheetId="2" r:id="rId2"/>
-    <sheet name="Obstacles" sheetId="3" r:id="rId3"/>
-    <sheet name="Cibles" sheetId="4" r:id="rId4"/>
-    <sheet name="Troupes" sheetId="5" r:id="rId5"/>
-    <sheet name="Dimensions" sheetId="6" r:id="rId6"/>
+    <sheet name="Dimensions" sheetId="6" r:id="rId1"/>
+    <sheet name="Troupes" sheetId="5" r:id="rId2"/>
+    <sheet name="Recrutement" sheetId="1" r:id="rId3"/>
+    <sheet name="Saboteurs" sheetId="2" r:id="rId4"/>
+    <sheet name="Obstacles" sheetId="3" r:id="rId5"/>
+    <sheet name="Influence" sheetId="4" r:id="rId6"/>
+    <sheet name="Ressources" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Dé</t>
   </si>
@@ -64,9 +65,6 @@
     <t>Saboteurs</t>
   </si>
   <si>
-    <t>Cibles</t>
-  </si>
-  <si>
     <t>7/joueurs</t>
   </si>
   <si>
@@ -101,6 +99,45 @@
   </si>
   <si>
     <t>d'un cercle</t>
+  </si>
+  <si>
+    <t>Donjons d'influence</t>
+  </si>
+  <si>
+    <t>Ressource</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>promontoire</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>forêt</t>
+  </si>
+  <si>
+    <t>Prairie</t>
+  </si>
+  <si>
+    <t>Mine</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Points totaux</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Frequence</t>
+  </si>
+  <si>
+    <t>NombrePrime</t>
   </si>
 </sst>
 </file>
@@ -111,7 +148,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +166,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -189,11 +233,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,11 +328,324 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -369,6 +788,30 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A1:G6" totalsRowCount="1" headerRowDxfId="12" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:G5" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="11" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="5">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/37</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="4">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="Frequence" dataDxfId="3" totalsRowDxfId="2">
+      <calculatedColumnFormula>1/(1+Tableau1[[#This Row],[Points]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" dataDxfId="1" totalsRowDxfId="0">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -633,6 +1076,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4EFBF6-12B3-45D8-B982-5090B8A756CF}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7">
+        <f>B1*B3</f>
+        <v>8.0829037686547593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8">
+        <f>2*SQRT(3)/3</f>
+        <v>1.1547005383792515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37527EB6-6690-4DE5-953A-72CFC0535AC8}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <f>37/B1*3</f>
+        <v>55.5</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:D4" si="0">37/C1*3</f>
+        <v>37</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>27.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <f>0.5*B4</f>
+        <v>27.75</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:D5" si="1">0.5*C4</f>
+        <v>18.5</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>13.875</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -732,12 +1326,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D52009-5336-40CE-B4E7-C4C0FDEEDFFC}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,11 +1369,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CA0E9F-C7C5-4402-B952-FCA0B456B247}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -801,7 +1395,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -818,15 +1412,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5686967-4540-41F3-AB14-90B6C2555286}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -844,7 +1441,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4">
         <v>4</v>
@@ -852,13 +1449,13 @@
       <c r="C2" s="5">
         <v>3</v>
       </c>
-      <c r="D2" s="6">
-        <v>2</v>
+      <c r="D2" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <f>7/B1</f>
@@ -878,153 +1475,176 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37527EB6-6690-4DE5-953A-72CFC0535AC8}">
-  <dimension ref="A1:D5"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C3F4A5-1DC5-4E3D-A691-49343372E105}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="2" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2" s="16">
+        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+        <v>0.1891891891891892</v>
+      </c>
+      <c r="E2" s="1">
+        <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3" s="16">
+        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+        <v>0.32432432432432434</v>
+      </c>
+      <c r="E3" s="1">
+        <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>12</v>
+      </c>
+      <c r="F3" s="1">
+        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="15">
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="16">
+        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+        <v>0.21621621621621623</v>
+      </c>
+      <c r="E4" s="1">
+        <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G4" s="15">
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="D1" s="3">
+      <c r="C5" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D5" s="16">
+        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="E5" s="1">
+        <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
+        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="15">
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5">
-        <v>20</v>
-      </c>
-      <c r="D2" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
-        <f>37/B1*3</f>
-        <v>55.5</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:D4" si="0">37/C1*3</f>
-        <v>37</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>27.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <f>0.5*B4</f>
-        <v>27.75</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" ref="C5:D5" si="1">0.5*C4</f>
-        <v>18.5</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>13.875</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4EFBF6-12B3-45D8-B982-5090B8A756CF}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="7">
-        <f>B1*B3</f>
-        <v>8.0829037686547593</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8">
-        <f>2*SQRT(3)/3</f>
-        <v>1.1547005383792515</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14">
+        <f>SUBTOTAL(109,Tableau1[Nombre])</f>
+        <v>31</v>
+      </c>
+      <c r="D6" s="17">
+        <f>SUBTOTAL(109,Tableau1[Ratio])</f>
+        <v>0.83783783783783794</v>
+      </c>
+      <c r="E6" s="14">
+        <f>SUBTOTAL(109,Tableau1[Points totaux])</f>
+        <v>40</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proposition de distribution de ressources
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3CF269-AF03-4083-9FFC-8CFAE06E55FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BA6752-A8FA-45AE-837E-D5AAD7AB2D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Dé</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Saboteurs</t>
   </si>
   <si>
-    <t>7/joueurs</t>
-  </si>
-  <si>
     <t>37/joueurs*3</t>
   </si>
   <si>
@@ -138,6 +135,24 @@
   </si>
   <si>
     <t>NombrePrime</t>
+  </si>
+  <si>
+    <t>FrequenceRelative</t>
+  </si>
+  <si>
+    <t>NombreMoyenTuilesPourDonjons</t>
+  </si>
+  <si>
+    <t>Donjons constructibles sans être adjacents sur les 37 tuiles</t>
+  </si>
+  <si>
+    <t>rien</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>à compter par paire</t>
   </si>
 </sst>
 </file>
@@ -178,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +224,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -294,12 +321,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -348,6 +410,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -355,73 +461,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -431,6 +471,23 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -443,6 +500,221 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -518,12 +790,31 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -533,6 +824,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -547,6 +839,74 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -568,6 +928,53 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -577,72 +984,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -791,24 +1132,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A1:G6" totalsRowCount="1" headerRowDxfId="12" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:G5" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="11" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A1:H7" totalsRowCount="1" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A1:H6" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="23" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="13">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="12">
       <calculatedColumnFormula>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="Frequence" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="FrequenceRelative" dataDxfId="19" totalsRowDxfId="11" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>1/(1+Tableau1[[#This Row],[Points]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" dataDxfId="1" totalsRowDxfId="0">
-      <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{67BBA106-5079-4C7C-8A22-2D09C9569940}" name="Frequence" dataDxfId="17" totalsRowDxfId="10" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>F2/SUM($F$2:$F$6)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="9">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*37</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}" name="Tableau2" displayName="Tableau2" ref="F14:I19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="F14:I19" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{ECDDF1B2-FC57-4D14-9CA2-B1F8DCB0128F}" name="Ressource" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1A596FA7-2330-4539-83A0-6561CBF106EF}" name="Nombre" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{5D189A14-ABCE-4B97-8187-B575326F4E1C}" name="Points" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C5740CE3-5BB3-4A90-AD40-CDF55C0B28F5}" name="Commentaire" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1090,7 +1447,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="7">
         <v>7</v>
@@ -1098,7 +1455,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="7">
         <f>B1*B3</f>
@@ -1107,7 +1464,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="8">
         <f>2*SQRT(3)/3</f>
@@ -1116,27 +1473,27 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1545,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <f>37/B1*3</f>
@@ -1205,7 +1562,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <f>0.5*B4</f>
@@ -1395,7 +1752,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -1414,10 +1771,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5686967-4540-41F3-AB14-90B6C2555286}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,33 +1798,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <f>7/B1</f>
-        <v>3.5</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ref="C4:D4" si="0">7/C1</f>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>1.75</v>
+        <v>18</v>
+      </c>
+      <c r="B2" s="23">
+        <v>2</v>
+      </c>
+      <c r="C2" s="23">
+        <v>2</v>
+      </c>
+      <c r="D2" s="23">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1477,102 +1817,115 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C3F4A5-1DC5-4E3D-A691-49343372E105}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="17" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="6" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B2" s="10">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>7</v>
-      </c>
-      <c r="D2" s="16">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.1891891891891892</v>
-      </c>
-      <c r="E2" s="1">
+        <v>0.27027027027027029</v>
+      </c>
+      <c r="E2" s="24">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>0</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="16">
         <f>1/(1+Tableau1[[#This Row],[Points]])</f>
         <v>1</v>
       </c>
-      <c r="G2" s="15">
-        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="25">
+        <f>F2/SUM($F$2:$F$6)</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="H2" s="2">
+        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <v>13.454545454545455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C3" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="16">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.32432432432432434</v>
+        <v>0.27027027027027029</v>
       </c>
       <c r="E3" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>12</v>
-      </c>
-      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="16">
         <f>1/(1+Tableau1[[#This Row],[Points]])</f>
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="15">
-        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G3" s="25">
+        <f t="shared" ref="G3:G6" si="0">F3/SUM($F$2:$F$6)</f>
+        <v>0.2424242424242424</v>
+      </c>
+      <c r="H3" s="2">
+        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <v>8.9696969696969688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
@@ -1583,25 +1936,29 @@
       </c>
       <c r="E4" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>16</v>
-      </c>
-      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="F4" s="16">
         <f>1/(1+Tableau1[[#This Row],[Points]])</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G4" s="15">
-        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>2.6666666666666665</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="13">
-        <v>3</v>
-      </c>
-      <c r="C5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="H4" s="2">
+        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <v>6.7272727272727275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="16">
@@ -1610,41 +1967,205 @@
       </c>
       <c r="E5" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
+        <v>8</v>
+      </c>
+      <c r="F5" s="16">
+        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1212121212121212</v>
+      </c>
+      <c r="H5" s="2">
+        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <v>4.4848484848484844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16">
+        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="E6" s="1">
+        <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>12</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="16">
         <f>1/(1+Tableau1[[#This Row],[Points]])</f>
         <v>0.25</v>
       </c>
-      <c r="G5" s="15">
-        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#This Row],[Nombre]]</f>
+      <c r="G6" s="25">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <v>3.3636363636363638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14">
+        <f>SUBTOTAL(109,Tableau1[Nombre])</f>
+        <v>36</v>
+      </c>
+      <c r="D7" s="17">
+        <f>SUBTOTAL(109,Tableau1[Ratio])</f>
+        <v>0.97297297297297303</v>
+      </c>
+      <c r="E7" s="14">
+        <f>SUBTOTAL(109,Tableau1[Points totaux])</f>
+        <v>33</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="18">
+        <f>SUBTOTAL(109,Tableau1[NombrePrime])</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="F14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="21">
+        <f>$A$12/A15</f>
+        <v>6</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="F15" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="26">
+        <v>10</v>
+      </c>
+      <c r="H15" s="26">
+        <v>0</v>
+      </c>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="21">
+        <f t="shared" ref="B16:B17" si="1">$A$12/A16</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="F16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="27">
+        <v>10</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="21">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="F17" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="26">
+        <v>8</v>
+      </c>
+      <c r="H17" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14">
-        <f>SUBTOTAL(109,Tableau1[Nombre])</f>
-        <v>31</v>
-      </c>
-      <c r="D6" s="17">
-        <f>SUBTOTAL(109,Tableau1[Ratio])</f>
-        <v>0.83783783783783794</v>
-      </c>
-      <c r="E6" s="14">
-        <f>SUBTOTAL(109,Tableau1[Points totaux])</f>
-        <v>40</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="27">
+        <v>4</v>
+      </c>
+      <c r="H18" s="27">
+        <v>2</v>
+      </c>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="32">
+        <v>4</v>
+      </c>
+      <c r="H19" s="32">
+        <v>3</v>
+      </c>
+      <c r="I19" s="33"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour des paramètres suite à test
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BA6752-A8FA-45AE-837E-D5AAD7AB2D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019F368E-4976-43D0-9588-D1E797E6FA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Dé</t>
   </si>
@@ -147,12 +147,6 @@
   </si>
   <si>
     <t>rien</t>
-  </si>
-  <si>
-    <t>Commentaire</t>
-  </si>
-  <si>
-    <t>à compter par paire</t>
   </si>
 </sst>
 </file>
@@ -237,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -329,28 +323,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -361,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,48 +384,32 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -461,45 +417,127 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -643,6 +681,25 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -650,6 +707,7 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -657,67 +715,18 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -729,64 +738,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -807,24 +761,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1132,25 +1068,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A1:H7" totalsRowCount="1" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A1:H7" totalsRowCount="1" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A1:H6" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="23" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="13">
+    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="22" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="4">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="12">
+    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="3">
       <calculatedColumnFormula>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="FrequenceRelative" dataDxfId="19" totalsRowDxfId="11" dataCellStyle="Pourcentage">
-      <calculatedColumnFormula>1/(1+Tableau1[[#This Row],[Points]])</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="FrequenceRelative" dataDxfId="18" totalsRowDxfId="2" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>1/(1+Tableau1[[#This Row],[Points]])^0.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67BBA106-5079-4C7C-8A22-2D09C9569940}" name="Frequence" dataDxfId="17" totalsRowDxfId="10" dataCellStyle="Pourcentage">
+    <tableColumn id="8" xr3:uid="{67BBA106-5079-4C7C-8A22-2D09C9569940}" name="Frequence" dataDxfId="17" totalsRowDxfId="1" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>F2/SUM($F$2:$F$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="9">
+    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="0">
       <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*37</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1159,13 +1095,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}" name="Tableau2" displayName="Tableau2" ref="F14:I19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="F14:I19" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECDDF1B2-FC57-4D14-9CA2-B1F8DCB0128F}" name="Ressource" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{1A596FA7-2330-4539-83A0-6561CBF106EF}" name="Nombre" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{5D189A14-ABCE-4B97-8187-B575326F4E1C}" name="Points" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C5740CE3-5BB3-4A90-AD40-CDF55C0B28F5}" name="Commentaire" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}" name="Tableau2" displayName="Tableau2" ref="F14:H19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="F14:H19" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{ECDDF1B2-FC57-4D14-9CA2-B1F8DCB0128F}" name="Ressource" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{1A596FA7-2330-4539-83A0-6561CBF106EF}" name="Nombre" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5D189A14-ABCE-4B97-8187-B575326F4E1C}" name="Points" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1800,13 +1735,13 @@
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="23">
-        <v>2</v>
-      </c>
-      <c r="C2" s="23">
-        <v>2</v>
-      </c>
-      <c r="D2" s="23">
+      <c r="B2" s="4">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1817,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C3F4A5-1DC5-4E3D-A691-49343372E105}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,11 +1763,10 @@
     <col min="1" max="2" width="17" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
@@ -1858,7 +1792,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
@@ -1866,195 +1800,195 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.27027027027027029</v>
-      </c>
-      <c r="E2" s="24">
+        <v>0.29729729729729731</v>
+      </c>
+      <c r="E2" s="20">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>0</v>
       </c>
       <c r="F2" s="16">
-        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
+        <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
         <v>1</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="16">
         <f>F2/SUM($F$2:$F$6)</f>
-        <v>0.36363636363636365</v>
+        <v>0.30943747354826506</v>
       </c>
       <c r="H2" s="2">
         <f>Tableau1[[#This Row],[Frequence]]*37</f>
-        <v>13.454545454545455</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11.449186521285807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="16">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.27027027027027029</v>
+        <v>0.21621621621621623</v>
       </c>
       <c r="E3" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3" s="16">
-        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G3" s="25">
+        <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="G3" s="16">
         <f t="shared" ref="G3:G6" si="0">F3/SUM($F$2:$F$6)</f>
-        <v>0.2424242424242424</v>
+        <v>0.21880533589921114</v>
       </c>
       <c r="H3" s="2">
         <f>Tableau1[[#This Row],[Frequence]]*37</f>
-        <v>8.9696969696969688</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8.0957974282708118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="16">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.21621621621621623</v>
+        <v>0.1891891891891892</v>
       </c>
       <c r="E4" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F4" s="16">
-        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="25">
+        <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G4" s="16">
         <f t="shared" si="0"/>
-        <v>0.18181818181818182</v>
+        <v>0.17865380865044855</v>
       </c>
       <c r="H4" s="2">
         <f>Tableau1[[#This Row],[Frequence]]*37</f>
-        <v>6.7272727272727275</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6.6101909200665965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="16">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.10810810810810811</v>
+        <v>0.16216216216216217</v>
       </c>
       <c r="E5" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F5" s="16">
-        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G5" s="25">
+        <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0.1212121212121212</v>
+        <v>0.15471873677413253</v>
       </c>
       <c r="H5" s="2">
         <f>Tableau1[[#This Row],[Frequence]]*37</f>
-        <v>4.4848484848484844</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5.7245932606429033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="16">
         <f>Tableau1[[#This Row],[Nombre]]/37</f>
-        <v>0.10810810810810811</v>
+        <v>0.13513513513513514</v>
       </c>
       <c r="E6" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F6" s="16">
-        <f>1/(1+Tableau1[[#This Row],[Points]])</f>
-        <v>0.25</v>
-      </c>
-      <c r="G6" s="25">
+        <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
+        <v>0.44721359549995793</v>
+      </c>
+      <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.13838464512794274</v>
       </c>
       <c r="H6" s="2">
         <f>Tableau1[[#This Row],[Frequence]]*37</f>
-        <v>3.3636363636363638</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5.1202318697338818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="14">
         <f>SUBTOTAL(109,Tableau1[Nombre])</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="17">
         <f>SUBTOTAL(109,Tableau1[Ratio])</f>
-        <v>0.97297297297297303</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="E7" s="14">
         <f>SUBTOTAL(109,Tableau1[Points totaux])</f>
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="18">
+      <c r="H7" s="2">
         <f>SUBTOTAL(109,Tableau1[NombrePrime])</f>
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="26"/>
       <c r="F14" s="11" t="s">
         <v>19</v>
       </c>
@@ -2064,95 +1998,85 @@
       <c r="H14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="27">
         <f>$A$12/A15</f>
         <v>6</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="F15" s="28" t="s">
+      <c r="C15" s="26"/>
+      <c r="F15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="26">
-        <v>10</v>
-      </c>
-      <c r="H15" s="26">
+      <c r="G15" s="21">
+        <v>11</v>
+      </c>
+      <c r="H15" s="21">
         <v>0</v>
       </c>
-      <c r="I15" s="24"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="27">
         <f t="shared" ref="B16:B17" si="1">$A$12/A16</f>
         <v>4</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="F16" s="29" t="s">
+      <c r="C16" s="26"/>
+      <c r="F16" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="27">
-        <v>10</v>
-      </c>
-      <c r="H16" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="F17" s="28" t="s">
+      <c r="C17" s="26"/>
+      <c r="F17" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="26">
-        <v>8</v>
-      </c>
-      <c r="H17" s="26">
-        <v>1</v>
-      </c>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="29" t="s">
+      <c r="G17" s="21">
+        <v>7</v>
+      </c>
+      <c r="H17" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="1">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="24">
+        <v>5</v>
+      </c>
+      <c r="H19" s="24">
         <v>4</v>
       </c>
-      <c r="H18" s="27">
-        <v>2</v>
-      </c>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="32">
-        <v>4</v>
-      </c>
-      <c r="H19" s="32">
-        <v>3</v>
-      </c>
-      <c r="I19" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
prise en compte des deux saboteurs dédiés
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019F368E-4976-43D0-9588-D1E797E6FA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2585C462-089A-4F12-9D7D-D68ED121D18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,7 +377,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,6 +409,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -437,53 +439,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -496,6 +451,57 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -538,6 +544,124 @@
           <color indexed="64"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -723,126 +847,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1073,21 +1077,21 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="7"/>
     <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="22" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="4">
-      <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/37</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Nombre" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{DA6BF02E-EF77-4DDC-8875-B686CBD20EC5}" name="Ratio" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="4" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="3">
+    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="3">
       <calculatedColumnFormula>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="FrequenceRelative" dataDxfId="18" totalsRowDxfId="2" dataCellStyle="Pourcentage">
+    <tableColumn id="6" xr3:uid="{F8C2F193-6B05-4294-AAA9-D0E833230C87}" name="FrequenceRelative" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>1/(1+Tableau1[[#This Row],[Points]])^0.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67BBA106-5079-4C7C-8A22-2D09C9569940}" name="Frequence" dataDxfId="17" totalsRowDxfId="1" dataCellStyle="Pourcentage">
-      <calculatedColumnFormula>F2/SUM($F$2:$F$6)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{67BBA106-5079-4C7C-8A22-2D09C9569940}" name="Frequence" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>F2/Tableau1[[#Totals],[FrequenceRelative]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="0">
-      <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*37</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{4A4AAE9E-7AB8-4C75-A3CD-F6C04C92724D}" name="NombrePrime" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="0">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*Tableau1[[#Totals],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1095,12 +1099,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}" name="Tableau2" displayName="Tableau2" ref="F14:H19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}" name="Tableau2" displayName="Tableau2" ref="F14:H19" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="F14:H19" xr:uid="{ADE94C2A-D1C3-4A6E-A312-6707F6367B20}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{ECDDF1B2-FC57-4D14-9CA2-B1F8DCB0128F}" name="Ressource" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{1A596FA7-2330-4539-83A0-6561CBF106EF}" name="Nombre" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{5D189A14-ABCE-4B97-8187-B575326F4E1C}" name="Points" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{ECDDF1B2-FC57-4D14-9CA2-B1F8DCB0128F}" name="Ressource" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{1A596FA7-2330-4539-83A0-6561CBF106EF}" name="Nombre" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{5D189A14-ABCE-4B97-8187-B575326F4E1C}" name="Points" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1741,7 +1745,7 @@
       <c r="C2" s="5">
         <v>3</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1755,7 +1759,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,24 +1806,24 @@
       <c r="C2" s="1">
         <v>11</v>
       </c>
-      <c r="D2" s="1">
-        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+      <c r="D2" s="15">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.29729729729729731</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="19">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>0</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
         <v>1</v>
       </c>
-      <c r="G2" s="16">
-        <f>F2/SUM($F$2:$F$6)</f>
+      <c r="G2" s="15">
+        <f>F2/Tableau1[[#Totals],[FrequenceRelative]]</f>
         <v>0.30943747354826506</v>
       </c>
       <c r="H2" s="2">
-        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#Totals],[Nombre]]</f>
         <v>11.449186521285807</v>
       </c>
     </row>
@@ -1833,24 +1837,24 @@
       <c r="C3" s="1">
         <v>8</v>
       </c>
-      <c r="D3" s="16">
-        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+      <c r="D3" s="15">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.21621621621621623</v>
       </c>
       <c r="E3" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>8</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
         <v>0.70710678118654746</v>
       </c>
-      <c r="G3" s="16">
-        <f t="shared" ref="G3:G6" si="0">F3/SUM($F$2:$F$6)</f>
+      <c r="G3" s="15">
+        <f>F3/Tableau1[[#Totals],[FrequenceRelative]]</f>
         <v>0.21880533589921114</v>
       </c>
       <c r="H3" s="2">
-        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#Totals],[Nombre]]</f>
         <v>8.0957974282708118</v>
       </c>
     </row>
@@ -1864,24 +1868,24 @@
       <c r="C4" s="1">
         <v>7</v>
       </c>
-      <c r="D4" s="16">
-        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+      <c r="D4" s="15">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.1891891891891892</v>
       </c>
       <c r="E4" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>14</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="G4" s="16">
-        <f t="shared" si="0"/>
+      <c r="G4" s="15">
+        <f>F4/Tableau1[[#Totals],[FrequenceRelative]]</f>
         <v>0.17865380865044855</v>
       </c>
       <c r="H4" s="2">
-        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#Totals],[Nombre]]</f>
         <v>6.6101909200665965</v>
       </c>
     </row>
@@ -1895,24 +1899,24 @@
       <c r="C5" s="1">
         <v>6</v>
       </c>
-      <c r="D5" s="16">
-        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+      <c r="D5" s="15">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.16216216216216217</v>
       </c>
       <c r="E5" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>18</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="15">
         <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
         <v>0.5</v>
       </c>
-      <c r="G5" s="16">
-        <f t="shared" si="0"/>
+      <c r="G5" s="15">
+        <f>F5/Tableau1[[#Totals],[FrequenceRelative]]</f>
         <v>0.15471873677413253</v>
       </c>
       <c r="H5" s="2">
-        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#Totals],[Nombre]]</f>
         <v>5.7245932606429033</v>
       </c>
     </row>
@@ -1926,24 +1930,24 @@
       <c r="C6" s="14">
         <v>5</v>
       </c>
-      <c r="D6" s="16">
-        <f>Tableau1[[#This Row],[Nombre]]/37</f>
+      <c r="D6" s="15">
+        <f>Tableau1[[#This Row],[Nombre]]/Tableau1[[#Totals],[Nombre]]</f>
         <v>0.13513513513513514</v>
       </c>
       <c r="E6" s="1">
         <f>Tableau1[[#This Row],[Points]]*Tableau1[[#This Row],[Nombre]]</f>
         <v>20</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <f>1/(1+Tableau1[[#This Row],[Points]])^0.5</f>
         <v>0.44721359549995793</v>
       </c>
-      <c r="G6" s="16">
-        <f t="shared" si="0"/>
+      <c r="G6" s="15">
+        <f>F6/Tableau1[[#Totals],[FrequenceRelative]]</f>
         <v>0.13838464512794274</v>
       </c>
       <c r="H6" s="2">
-        <f>Tableau1[[#This Row],[Frequence]]*37</f>
+        <f>Tableau1[[#This Row],[Frequence]]*Tableau1[[#Totals],[Nombre]]</f>
         <v>5.1202318697338818</v>
       </c>
     </row>
@@ -1956,7 +1960,7 @@
         <f>SUBTOTAL(109,Tableau1[Nombre])</f>
         <v>37</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <f>SUBTOTAL(109,Tableau1[Ratio])</f>
         <v>1.0000000000000002</v>
       </c>
@@ -1964,8 +1968,14 @@
         <f>SUBTOTAL(109,Tableau1[Points totaux])</f>
         <v>60</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="27">
+        <f>SUBTOTAL(109,Tableau1[FrequenceRelative])</f>
+        <v>3.2316706458761311</v>
+      </c>
+      <c r="G7" s="27">
+        <f>SUBTOTAL(109,Tableau1[Frequence])</f>
+        <v>1</v>
+      </c>
       <c r="H7" s="2">
         <f>SUBTOTAL(109,Tableau1[NombrePrime])</f>
         <v>37</v>
@@ -1982,13 +1992,13 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="25"/>
       <c r="F14" s="11" t="s">
         <v>19</v>
       </c>
@@ -2003,18 +2013,18 @@
       <c r="A15" s="1">
         <v>2</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="26">
         <f>$A$12/A15</f>
         <v>6</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="F15" s="22" t="s">
+      <c r="C15" s="25"/>
+      <c r="F15" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="20">
         <v>11</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="20">
         <v>0</v>
       </c>
     </row>
@@ -2022,11 +2032,11 @@
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="27">
-        <f t="shared" ref="B16:B17" si="1">$A$12/A16</f>
+      <c r="B16" s="26">
+        <f t="shared" ref="B16:B17" si="0">$A$12/A16</f>
         <v>4</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="25"/>
       <c r="F16" s="10" t="s">
         <v>21</v>
       </c>
@@ -2041,18 +2051,18 @@
       <c r="A17" s="1">
         <v>4</v>
       </c>
-      <c r="B17" s="27">
-        <f t="shared" si="1"/>
+      <c r="B17" s="26">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="F17" s="22" t="s">
+      <c r="C17" s="25"/>
+      <c r="F17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>7</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="20">
         <v>2</v>
       </c>
     </row>
@@ -2068,13 +2078,13 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="23">
         <v>5</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="23">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout des statistiques sur le système de points
</commit_message>
<xml_diff>
--- a/Parametres.xlsx
+++ b/Parametres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandre\Documents\GitHub\Donjons-et-Barons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1A6D18-3BF3-4F99-B93B-02D1FADE34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B850CF-052A-42D7-B27E-6A2E25F9927A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Dé</t>
   </si>
@@ -158,7 +158,25 @@
     <t>SommePoints</t>
   </si>
   <si>
-    <t>Simple</t>
+    <t>Binaire</t>
+  </si>
+  <si>
+    <t>Ternaire</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>Quaternaire</t>
+  </si>
+  <si>
+    <t>r4</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,10 +497,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,35 +517,709 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+  <dxfs count="108">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -557,49 +1258,85 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -633,12 +1370,22 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -657,56 +1404,13 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -714,12 +1418,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -729,18 +1429,42 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -748,76 +1472,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1913,26 +2567,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A2:I8" totalsRowCount="1" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}" name="Tableau1" displayName="Tableau1" ref="A2:I8" totalsRowCount="1" headerRowDxfId="107" headerRowBorderDxfId="106" tableBorderDxfId="105" totalsRowBorderDxfId="104">
   <autoFilter ref="A2:I7" xr:uid="{7199411E-CFFA-4600-AB44-E5BC1C3DE055}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{73FFCB6D-C942-4B7B-9EC1-70102A1FBDF7}" name="Rang" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{5DA34DB0-ECB6-4CCD-8C55-D6EB555280F2}" name="FrequenceRelative" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56" dataCellStyle="Pourcentage">
+    <tableColumn id="1" xr3:uid="{F858E9F4-AE96-4C5D-8D22-2620CFF6B1D1}" name="Ressource" totalsRowLabel="Total" dataDxfId="103" totalsRowDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{05EE0077-D79F-4016-9586-36C2ADD08490}" name="Points" dataDxfId="101" totalsRowDxfId="100"/>
+    <tableColumn id="9" xr3:uid="{73FFCB6D-C942-4B7B-9EC1-70102A1FBDF7}" name="Rang" dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="10" xr3:uid="{5DA34DB0-ECB6-4CCD-8C55-D6EB555280F2}" name="FrequenceRelative" totalsRowFunction="sum" dataDxfId="97" totalsRowDxfId="96" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>1/Tableau1[[#This Row],[Rang]]^1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Frequence" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54">
+    <tableColumn id="2" xr3:uid="{F1384E0B-F0E5-4670-B89E-EF5705088279}" name="Frequence" totalsRowFunction="sum" dataDxfId="95" totalsRowDxfId="94">
       <calculatedColumnFormula>Tableau1[[#This Row],[FrequenceRelative]]/SUM(Tableau1[FrequenceRelative])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FA35D35B-401E-4AEC-BE35-C2CAC4718886}" name="NombreReel" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52" dataCellStyle="Pourcentage">
+    <tableColumn id="11" xr3:uid="{FA35D35B-401E-4AEC-BE35-C2CAC4718886}" name="NombreReel" totalsRowFunction="sum" dataDxfId="93" totalsRowDxfId="92" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau1[[#This Row],[Frequence]]*37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux reels" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50">
+    <tableColumn id="5" xr3:uid="{174EBAF5-0C68-4E81-BBFE-03B8E207101A}" name="Points totaux reels" totalsRowFunction="sum" dataDxfId="91" totalsRowDxfId="90">
       <calculatedColumnFormula>Tableau1[[#This Row],[NombreReel]]*Tableau1[[#This Row],[Points]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{AD1C73DB-125E-496E-BF9A-C50E00C25BF2}" name="Nombre" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="13" xr3:uid="{EEBBC92F-CECA-4B9B-B45B-D321EA3D9EBF}" name="Points totaux" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46">
+    <tableColumn id="12" xr3:uid="{AD1C73DB-125E-496E-BF9A-C50E00C25BF2}" name="Nombre" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="13" xr3:uid="{EEBBC92F-CECA-4B9B-B45B-D321EA3D9EBF}" name="Points totaux" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="86">
       <calculatedColumnFormula>Tableau1[[#This Row],[Nombre]]*Tableau1[[#This Row],[Points]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1941,16 +2595,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4341CC7-DBF2-4D70-946D-C37644788646}" name="Tableau2" displayName="Tableau2" ref="A12:E18" totalsRowCount="1" headerRowDxfId="45" dataDxfId="43" totalsRowDxfId="41" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4341CC7-DBF2-4D70-946D-C37644788646}" name="Tableau2" displayName="Tableau2" ref="A12:E18" totalsRowCount="1" headerRowDxfId="85" dataDxfId="83" totalsRowDxfId="81" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="80">
   <autoFilter ref="A12:E17" xr:uid="{C4341CC7-DBF2-4D70-946D-C37644788646}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C5073434-1158-41DA-83D2-EAD365A35297}" name="Ressource" totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{E5857478-C1B5-4E3D-BC07-FACDAE90FD78}" name="Points" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{476A896F-4787-40FB-A2BC-927386B0C9EF}" name="Nombre" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{49DCB62C-1427-4E4F-B357-F1A9C97DE0A3}" name="Frequence" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Pourcentage">
+    <tableColumn id="1" xr3:uid="{C5073434-1158-41DA-83D2-EAD365A35297}" name="Ressource" totalsRowLabel="Total" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{E5857478-C1B5-4E3D-BC07-FACDAE90FD78}" name="Points" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{476A896F-4787-40FB-A2BC-927386B0C9EF}" name="Nombre" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{49DCB62C-1427-4E4F-B357-F1A9C97DE0A3}" name="Frequence" totalsRowFunction="sum" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau2[[#This Row],[Nombre]]/Tableau2[[#Totals],[Nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{76BC6A54-9D20-4F99-BBA3-549440205E76}" name="Points totaux" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="5" xr3:uid="{76BC6A54-9D20-4F99-BBA3-549440205E76}" name="Points totaux" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70">
       <calculatedColumnFormula>Tableau2[[#This Row],[Nombre]]*Tableau2[[#This Row],[Points]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1959,35 +2613,83 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5636E3E1-FB8C-4D6D-854E-7510C85A4B47}" name="Tableau3" displayName="Tableau3" ref="A22:C28" totalsRowCount="1" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5636E3E1-FB8C-4D6D-854E-7510C85A4B47}" name="Tableau3" displayName="Tableau3" ref="A22:C28" totalsRowCount="1" headerRowDxfId="69" headerRowBorderDxfId="68" tableBorderDxfId="67" totalsRowBorderDxfId="66">
   <autoFilter ref="A22:C27" xr:uid="{5636E3E1-FB8C-4D6D-854E-7510C85A4B47}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1968D85F-B0B8-41E7-8CFF-5978F4FE1E62}" name="Ressource" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{7FF1C41F-572F-4877-9D2F-CAAEF911E38D}" name="Points" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{6CE2C703-3FA2-4CAF-BB9A-BDD7F84057DF}" name="Nombre" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{1968D85F-B0B8-41E7-8CFF-5978F4FE1E62}" name="Ressource" totalsRowLabel="Total" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{7FF1C41F-572F-4877-9D2F-CAAEF911E38D}" name="Points" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{6CE2C703-3FA2-4CAF-BB9A-BDD7F84057DF}" name="Nombre" totalsRowFunction="sum" dataDxfId="61" totalsRowDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{089AEE7E-4AB5-4382-83BF-74544EE123B2}" name="Tableau5" displayName="Tableau5" ref="A32:G35" totalsRowCount="1" headerRowDxfId="15" dataDxfId="19" totalsRowDxfId="14" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{089AEE7E-4AB5-4382-83BF-74544EE123B2}" name="Tableau5" displayName="Tableau5" ref="A32:G35" totalsRowCount="1" headerRowDxfId="59" dataDxfId="57" totalsRowDxfId="55" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="54">
   <autoFilter ref="A32:G34" xr:uid="{089AEE7E-4AB5-4382-83BF-74544EE123B2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BEF3ED4B-8C14-49FB-9250-C627BF3DE4D2}" name="Ressource" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{61B8AEC7-86FE-4697-93D1-763B488FD723}" name="Points" dataDxfId="12" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{819389B4-25A1-4331-84BA-6C347D64278B}" name="Rang" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{09B8AF64-8A4B-4DB9-8CCB-BC99E80C370D}" name="NombreRelatif" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="3">
+    <tableColumn id="1" xr3:uid="{BEF3ED4B-8C14-49FB-9250-C627BF3DE4D2}" name="Ressource" totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{61B8AEC7-86FE-4697-93D1-763B488FD723}" name="Points" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{819389B4-25A1-4331-84BA-6C347D64278B}" name="Rang" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{09B8AF64-8A4B-4DB9-8CCB-BC99E80C370D}" name="NombreRelatif" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46">
       <calculatedColumnFormula>1/Tableau5[[#This Row],[Rang]]^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4187A737-7549-4422-BB2B-560E5A1D7E2E}" name="Fréquence" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2" dataCellStyle="Pourcentage">
+    <tableColumn id="5" xr3:uid="{4187A737-7549-4422-BB2B-560E5A1D7E2E}" name="Fréquence" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau5[[#This Row],[NombreRelatif]]/Tableau5[[#Totals],[NombreRelatif]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{90BE00BA-725D-4605-A197-781633525FBC}" name="Nombre" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1">
+    <tableColumn id="6" xr3:uid="{90BE00BA-725D-4605-A197-781633525FBC}" name="Nombre" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>ROUND(Tableau5[[#This Row],[Fréquence]]*37,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7BF2BAB6-A961-40D7-AE96-7BDC6A103D30}" name="SommePoints" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{7BF2BAB6-A961-40D7-AE96-7BDC6A103D30}" name="SommePoints" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>Tableau5[[#This Row],[Nombre]]*Tableau5[[#This Row],[Points]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{06C4A83B-FC0F-40FF-AC4A-A2BD6C60C871}" name="Tableau55" displayName="Tableau55" ref="A38:G42" totalsRowCount="1" headerRowDxfId="39" dataDxfId="37" totalsRowDxfId="35" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="34">
+  <autoFilter ref="A38:G41" xr:uid="{06C4A83B-FC0F-40FF-AC4A-A2BD6C60C871}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{57259079-2BFB-4626-99F0-67DB5832B318}" name="Ressource" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{05BFC6A6-C1B4-4DE5-97B3-3FA82E19E428}" name="Points" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{31DFCB04-F660-4E4F-B423-7C1D0703597B}" name="Rang" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{382F5270-7E39-408A-A234-9568A0EE9EE2}" name="NombreRelatif" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
+      <calculatedColumnFormula>1/Tableau55[[#This Row],[Rang]]^2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{2A0E97CF-95FE-410E-9402-FCD172E44A78}" name="Fréquence" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>Tableau55[[#This Row],[NombreRelatif]]/Tableau55[[#Totals],[NombreRelatif]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{740AF54D-5406-4197-9877-0D01C1AE0D66}" name="Nombre" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22">
+      <calculatedColumnFormula>ROUND(Tableau55[[#This Row],[Fréquence]]*37,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{EDAAEF34-5F95-40A3-AF8A-9310D3045659}" name="SommePoints" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20">
+      <calculatedColumnFormula>Tableau55[[#This Row],[Nombre]]*Tableau55[[#This Row],[Points]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C221EC22-E8F7-4257-B235-459AC9677D12}" name="Tableau557" displayName="Tableau557" ref="A46:G51" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18" totalsRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+  <autoFilter ref="A46:G50" xr:uid="{C221EC22-E8F7-4257-B235-459AC9677D12}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{9168696D-A16F-42E9-93BE-3BFEFA8EDEF0}" name="Ressource" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6CEE42E6-4FD0-49AE-B1A2-48FDCA7D4E95}" name="Points" dataDxfId="12" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{015E657B-857D-4CA8-A2B5-A582C81E5B33}" name="Rang" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{2ADA9829-8EA4-40EC-A763-D9C7D814F3D2}" name="NombreRelatif" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="3">
+      <calculatedColumnFormula>1/Tableau557[[#This Row],[Rang]]^2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{605DAA4C-1435-461D-953D-A4DB62FEEEFC}" name="Fréquence" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2" dataCellStyle="Pourcentage">
+      <calculatedColumnFormula>Tableau557[[#This Row],[NombreRelatif]]/Tableau557[[#Totals],[NombreRelatif]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{77758C45-8534-4499-B8AD-9789C309A769}" name="Nombre" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1">
+      <calculatedColumnFormula>ROUND(Tableau557[[#This Row],[Fréquence]]*37,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{AF7B9E32-E404-4771-A9AE-CAD0963718B8}" name="SommePoints" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="0">
+      <calculatedColumnFormula>Tableau557[[#This Row],[Nombre]]*Tableau557[[#This Row],[Points]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2427,10 +3129,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C3F4A5-1DC5-4E3D-A691-49343372E105}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3005,15 +3707,314 @@
         <v>44</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7">
+        <f>1/Tableau55[[#This Row],[Rang]]^2</f>
+        <v>1</v>
+      </c>
+      <c r="E39" s="30">
+        <f>Tableau55[[#This Row],[NombreRelatif]]/Tableau55[[#Totals],[NombreRelatif]]</f>
+        <v>0.73469387755102034</v>
+      </c>
+      <c r="F39" s="36">
+        <f>ROUND(Tableau55[[#This Row],[Fréquence]]*37,0)</f>
+        <v>27</v>
+      </c>
+      <c r="G39" s="1">
+        <f>Tableau55[[#This Row],[Nombre]]*Tableau55[[#This Row],[Points]]</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="7">
+        <f>1/Tableau55[[#This Row],[Rang]]^2</f>
+        <v>0.25</v>
+      </c>
+      <c r="E40" s="30">
+        <f>Tableau55[[#This Row],[NombreRelatif]]/Tableau55[[#Totals],[NombreRelatif]]</f>
+        <v>0.18367346938775508</v>
+      </c>
+      <c r="F40" s="36">
+        <f>ROUND(Tableau55[[#This Row],[Fréquence]]*37,0)</f>
+        <v>7</v>
+      </c>
+      <c r="G40" s="1">
+        <f>Tableau55[[#This Row],[Nombre]]*Tableau55[[#This Row],[Points]]</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="13">
+        <v>3</v>
+      </c>
+      <c r="C41" s="13">
+        <v>3</v>
+      </c>
+      <c r="D41" s="39">
+        <f>1/Tableau55[[#This Row],[Rang]]^2</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E41" s="37">
+        <f>Tableau55[[#This Row],[NombreRelatif]]/Tableau55[[#Totals],[NombreRelatif]]</f>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="F41" s="38">
+        <f>ROUND(Tableau55[[#This Row],[Fréquence]]*37,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G41" s="13">
+        <f>Tableau55[[#This Row],[Nombre]]*Tableau55[[#This Row],[Points]]</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13">
+        <f>SUBTOTAL(109,Tableau55[Rang])</f>
+        <v>6</v>
+      </c>
+      <c r="D42" s="39">
+        <f>SUBTOTAL(109,Tableau55[NombreRelatif])</f>
+        <v>1.3611111111111112</v>
+      </c>
+      <c r="E42" s="35">
+        <f>SUBTOTAL(109,Tableau55[Fréquence])</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="F42" s="13">
+        <f>SUBTOTAL(109,Tableau55[Nombre])</f>
+        <v>37</v>
+      </c>
+      <c r="G42" s="13">
+        <f>SUBTOTAL(109,Tableau55[SommePoints])</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="7">
+        <f>1/Tableau557[[#This Row],[Rang]]^2</f>
+        <v>1</v>
+      </c>
+      <c r="E47" s="30">
+        <f>Tableau557[[#This Row],[NombreRelatif]]/Tableau557[[#Totals],[NombreRelatif]]</f>
+        <v>0.70243902439024386</v>
+      </c>
+      <c r="F47" s="36">
+        <f>ROUND(Tableau557[[#This Row],[Fréquence]]*37,0)</f>
+        <v>26</v>
+      </c>
+      <c r="G47" s="1">
+        <f>Tableau557[[#This Row],[Nombre]]*Tableau557[[#This Row],[Points]]</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="7">
+        <f>1/Tableau557[[#This Row],[Rang]]^2</f>
+        <v>0.25</v>
+      </c>
+      <c r="E48" s="30">
+        <f>Tableau557[[#This Row],[NombreRelatif]]/Tableau557[[#Totals],[NombreRelatif]]</f>
+        <v>0.17560975609756097</v>
+      </c>
+      <c r="F48" s="36">
+        <f>ROUND(Tableau557[[#This Row],[Fréquence]]*37,0)</f>
+        <v>6</v>
+      </c>
+      <c r="G48" s="1">
+        <f>Tableau557[[#This Row],[Nombre]]*Tableau557[[#This Row],[Points]]</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="13">
+        <v>3</v>
+      </c>
+      <c r="C49" s="13">
+        <v>3</v>
+      </c>
+      <c r="D49" s="39">
+        <f>1/Tableau557[[#This Row],[Rang]]^2</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E49" s="37">
+        <f>Tableau557[[#This Row],[NombreRelatif]]/Tableau557[[#Totals],[NombreRelatif]]</f>
+        <v>7.8048780487804864E-2</v>
+      </c>
+      <c r="F49" s="38">
+        <f>ROUND(Tableau557[[#This Row],[Fréquence]]*37,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G49" s="13">
+        <f>Tableau557[[#This Row],[Nombre]]*Tableau557[[#This Row],[Points]]</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="1">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>4</v>
+      </c>
+      <c r="D50" s="39">
+        <f>1/Tableau557[[#This Row],[Rang]]^2</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E50" s="37">
+        <f>Tableau557[[#This Row],[NombreRelatif]]/Tableau557[[#Totals],[NombreRelatif]]</f>
+        <v>4.3902439024390241E-2</v>
+      </c>
+      <c r="F50" s="38">
+        <f>ROUND(Tableau557[[#This Row],[Fréquence]]*37,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G50" s="13">
+        <f>Tableau557[[#This Row],[Nombre]]*Tableau557[[#This Row],[Points]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13">
+        <f>SUBTOTAL(109,Tableau557[Rang])</f>
+        <v>10</v>
+      </c>
+      <c r="D51" s="39">
+        <f>SUBTOTAL(109,Tableau557[NombreRelatif])</f>
+        <v>1.4236111111111112</v>
+      </c>
+      <c r="E51" s="35">
+        <f>SUBTOTAL(109,Tableau557[Fréquence])</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="F51" s="13">
+        <f>SUBTOTAL(109,Tableau557[Nombre])</f>
+        <v>37</v>
+      </c>
+      <c r="G51" s="13">
+        <f>SUBTOTAL(109,Tableau557[SommePoints])</f>
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>